<commit_message>
update plan week 4
</commit_message>
<xml_diff>
--- a/1.Plan/KẾ HOẠCH TUẦN.xlsx
+++ b/1.Plan/KẾ HOẠCH TUẦN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GAME\GAME-AI LA TRIEU PHU\1.Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847500E6-AAAD-490C-B6CC-023217E1DEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3E95B-39D9-4F1B-BC20-F08A6B98A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17115" yWindow="780" windowWidth="7500" windowHeight="6000" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
   </bookViews>
   <sheets>
     <sheet name="KẾ HOẠCH" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Loại công việc</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Ngày hoàn thành</t>
   </si>
   <si>
-    <t>02.Đang thực hiện</t>
-  </si>
-  <si>
     <t>03.Đã hoàn thành</t>
   </si>
   <si>
@@ -147,7 +144,40 @@
     <t>Design doc phần 4</t>
   </si>
   <si>
-    <t>Tuần 4-5</t>
+    <t>Tuần 4</t>
+  </si>
+  <si>
+    <t>TK.08</t>
+  </si>
+  <si>
+    <t>TK.09</t>
+  </si>
+  <si>
+    <t>TK.10</t>
+  </si>
+  <si>
+    <t>Design doc phần 5</t>
+  </si>
+  <si>
+    <t>Design doc phần 6</t>
+  </si>
+  <si>
+    <t>Design doc phần 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiện </t>
+  </si>
+  <si>
+    <t>01.Chưa thực hiện</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện</t>
+  </si>
+  <si>
+    <t>UI.01</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện màn hình game</t>
   </si>
 </sst>
 </file>
@@ -825,14 +855,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39B6E46-A377-4409-85DC-85EF42CEDBC4}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
@@ -845,16 +875,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -877,7 +907,7 @@
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -894,16 +924,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="F3" s="8">
         <v>45243</v>
@@ -912,7 +942,7 @@
         <v>45249</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="8">
         <v>45249</v>
@@ -921,7 +951,7 @@
     </row>
     <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -938,16 +968,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F5" s="8">
         <v>45257</v>
@@ -956,7 +986,7 @@
         <v>45260</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5" s="8">
         <v>45260</v>
@@ -968,16 +998,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="8">
         <v>45257</v>
@@ -986,7 +1016,7 @@
         <v>45260</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="8">
         <v>45259</v>
@@ -998,16 +1028,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8">
         <v>45257</v>
@@ -1016,9 +1046,11 @@
         <v>45260</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="I7" s="8">
+        <v>45260</v>
+      </c>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1026,16 +1058,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="8">
         <v>45252</v>
@@ -1044,7 +1076,7 @@
         <v>45263</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" s="8">
         <v>45260</v>
@@ -1056,16 +1088,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8">
         <v>45252</v>
@@ -1074,7 +1106,7 @@
         <v>45263</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" s="8">
         <v>45258</v>
@@ -1086,16 +1118,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="8">
         <v>45252</v>
@@ -1106,7 +1138,9 @@
       <c r="H10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8">
+        <v>45261</v>
+      </c>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1114,16 +1148,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="8">
         <v>45252</v>
@@ -1132,7 +1166,7 @@
         <v>45263</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" s="8">
         <v>45258</v>
@@ -1141,7 +1175,7 @@
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1157,13 +1191,27 @@
       <c r="A13" s="4">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="8">
+        <v>45264</v>
+      </c>
+      <c r="G13" s="8">
+        <v>45270</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="10"/>
     </row>
@@ -1171,13 +1219,27 @@
       <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="8">
+        <v>45264</v>
+      </c>
+      <c r="G14" s="8">
+        <v>45270</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I14" s="8"/>
       <c r="J14" s="10"/>
     </row>
@@ -1185,27 +1247,55 @@
       <c r="A15" s="4">
         <v>10</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="8">
+        <v>45264</v>
+      </c>
+      <c r="G15" s="8">
+        <v>45270</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="I15" s="8"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>11</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="8">
+        <v>45264</v>
+      </c>
+      <c r="G16" s="8">
+        <v>45270</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="10"/>
     </row>

</xml_diff>

<commit_message>
update plan week 5
</commit_message>
<xml_diff>
--- a/1.Plan/KẾ HOẠCH TUẦN.xlsx
+++ b/1.Plan/KẾ HOẠCH TUẦN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GAME\GAME-AI LA TRIEU PHU\1.Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C3E95B-39D9-4F1B-BC20-F08A6B98A2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91410629-CD03-4FCD-8C6A-6B078DD5C1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
+    <workbookView xWindow="17595" yWindow="5085" windowWidth="7500" windowHeight="6000" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
   </bookViews>
   <sheets>
     <sheet name="KẾ HOẠCH" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Loại công việc</t>
   </si>
@@ -168,9 +168,6 @@
     <t xml:space="preserve">Thiện </t>
   </si>
   <si>
-    <t>01.Chưa thực hiện</t>
-  </si>
-  <si>
     <t>Thiết kế giao diện</t>
   </si>
   <si>
@@ -178,6 +175,48 @@
   </si>
   <si>
     <t>Thiết kế giao diện màn hình game</t>
+  </si>
+  <si>
+    <t>02.Đang thực hiện</t>
+  </si>
+  <si>
+    <t>Phát triển game</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>Tuần 5-6-7</t>
+  </si>
+  <si>
+    <t>Tìm kiếm danh sách câu hỏi</t>
+  </si>
+  <si>
+    <t>Tìm Asset cho game</t>
+  </si>
+  <si>
+    <t>Chức năng trả lời câu hỏi</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>Chuyển các màn hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trình </t>
   </si>
 </sst>
 </file>
@@ -189,7 +228,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]d/mmm/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +244,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -324,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -365,11 +410,63 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -853,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39B6E46-A377-4409-85DC-85EF42CEDBC4}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +961,7 @@
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
@@ -1210,9 +1307,11 @@
         <v>45270</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="I13" s="8">
+        <v>45269</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1238,9 +1337,11 @@
         <v>45270</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="I14" s="8">
+        <v>45270</v>
+      </c>
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1266,23 +1367,25 @@
         <v>45270</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="I15" s="8">
+        <v>45269</v>
+      </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>31</v>
@@ -1296,85 +1399,147 @@
       <c r="H16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="8">
+        <v>45264</v>
+      </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>12</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8">
+        <v>45271</v>
+      </c>
+      <c r="G18" s="8">
+        <v>45278</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="I18" s="8"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>14</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="8">
+        <v>45271</v>
+      </c>
+      <c r="G19" s="8">
+        <v>45278</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="I19" s="8"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>15</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="8">
+        <v>45271</v>
+      </c>
+      <c r="G20" s="8">
+        <v>45278</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="I20" s="8"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>16</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="8">
+        <v>45271</v>
+      </c>
+      <c r="G21" s="8">
+        <v>45278</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="I21" s="8"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>17</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
@@ -1383,13 +1548,54 @@
       <c r="I22" s="8"/>
       <c r="J22" s="10"/>
     </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>17</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+      <formula>"04.Không thực hiện"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+      <formula>"03.Đã hoàn thành"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>"02.Đang thực hiện"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"Đã xong FS, chưa review KH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+      <formula>"KH đã confirm thiết kế"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1 C5">
+    <cfRule type="duplicateValues" dxfId="20" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H11 H13:H16 H19:H23">
     <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>"04.Không thực hiện"</formula>
     </cfRule>
@@ -1400,7 +1606,7 @@
       <formula>"02.Đang thực hiện"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
+  <conditionalFormatting sqref="J6:J11 J13:J16 J19:J23">
     <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Đã xong FS, chưa review KH"</formula>
     </cfRule>
@@ -1408,38 +1614,38 @@
       <formula>"KH đã confirm thiết kế"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 C5">
-    <cfRule type="duplicateValues" dxfId="14" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H11 H13:H22">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
-      <formula>"04.Không thực hiện"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
-      <formula>"03.Đã hoàn thành"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"02.Đang thực hiện"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J6:J11 J13:J22">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Đã xong FS, chưa review KH"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
-      <formula>"KH đã confirm thiết kế"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C8 C11 C13:C22">
-    <cfRule type="duplicateValues" dxfId="8" priority="14"/>
+  <conditionalFormatting sqref="C6:C8 C11 C13:C16 C19:C23">
+    <cfRule type="duplicateValues" dxfId="14" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"04.Không thực hiện"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"03.Đã hoàn thành"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"02.Đang thực hiện"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Đã xong FS, chưa review KH"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"KH đã confirm thiết kế"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"04.Không thực hiện"</formula>
     </cfRule>
@@ -1450,7 +1656,7 @@
       <formula>"02.Đang thực hiện"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3">
+  <conditionalFormatting sqref="J18">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Đã xong FS, chưa review KH"</formula>
     </cfRule>
@@ -1458,11 +1664,11 @@
       <formula>"KH đã confirm thiết kế"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
+  <conditionalFormatting sqref="C18">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H11 H13:H22" xr:uid="{B49D24C4-631E-43E3-86B9-0A25F3615237}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H11 H13:H16 H18:H23" xr:uid="{B49D24C4-631E-43E3-86B9-0A25F3615237}">
       <formula1>"01.Chưa thực hiện, 02.Đang thực hiện, 03.Đã hoàn thành, 04.Không thực hiện"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update plan week 6
</commit_message>
<xml_diff>
--- a/1.Plan/KẾ HOẠCH TUẦN.xlsx
+++ b/1.Plan/KẾ HOẠCH TUẦN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GAME\GAME-AI LA TRIEU PHU\1.Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91410629-CD03-4FCD-8C6A-6B078DD5C1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3D60BC-BB26-4772-98E9-06431B6717C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17595" yWindow="5085" windowWidth="7500" windowHeight="6000" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
+    <workbookView xWindow="7425" yWindow="780" windowWidth="20145" windowHeight="10275" xr2:uid="{46CEC522-137B-4F22-ACDE-89B13CE9558D}"/>
   </bookViews>
   <sheets>
     <sheet name="KẾ HOẠCH" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Loại công việc</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Thiết kế giao diện màn hình game</t>
-  </si>
-  <si>
-    <t>02.Đang thực hiện</t>
   </si>
   <si>
     <t>Phát triển game</t>
@@ -401,6 +398,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -410,7 +408,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39B6E46-A377-4409-85DC-85EF42CEDBC4}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,18 +1000,18 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -1047,18 +1044,18 @@
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1271,18 +1268,18 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -1405,31 +1402,31 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
+      <c r="A17" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>15</v>
@@ -1451,13 +1448,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>23</v>
@@ -1469,7 +1466,7 @@
         <v>45278</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="10"/>
@@ -1479,16 +1476,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="8">
         <v>45271</v>
@@ -1497,7 +1494,7 @@
         <v>45278</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="10"/>
@@ -1507,13 +1504,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>25</v>
@@ -1525,7 +1522,7 @@
         <v>45278</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="10"/>
@@ -1535,10 +1532,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
@@ -1553,10 +1550,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>

</xml_diff>